<commit_message>
update after ZP S1 raw file correction
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/PLITs/2-Relative_cover_category/plits_ext_df.xlsx
+++ b/Multi-taxa_data/PLITs/2-Relative_cover_category/plits_ext_df.xlsx
@@ -26552,10 +26552,10 @@
         </is>
       </c>
       <c r="B596">
-        <v>0</v>
+        <v>1469</v>
       </c>
       <c r="C596">
-        <v>0</v>
+        <v>0.596</v>
       </c>
       <c r="D596" t="inlineStr">
         <is>
@@ -26586,7 +26586,7 @@
         <v>1</v>
       </c>
       <c r="J596">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="597">
@@ -26643,7 +26643,7 @@
         <v>956</v>
       </c>
       <c r="C598">
-        <v>0.965</v>
+        <v>0.388</v>
       </c>
       <c r="D598" t="inlineStr">
         <is>
@@ -26674,7 +26674,7 @@
         <v>1</v>
       </c>
       <c r="J598">
-        <v>0.31</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="599">
@@ -26860,10 +26860,10 @@
         </is>
       </c>
       <c r="B603">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C603">
-        <v>0.027</v>
+        <v>0.012</v>
       </c>
       <c r="D603" t="inlineStr">
         <is>
@@ -26907,7 +26907,7 @@
         <v>8</v>
       </c>
       <c r="C604">
-        <v>0.008</v>
+        <v>0.003</v>
       </c>
       <c r="D604" t="inlineStr">
         <is>
@@ -26982,7 +26982,7 @@
         <v>2</v>
       </c>
       <c r="J605">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="606">
@@ -27070,7 +27070,7 @@
         <v>2</v>
       </c>
       <c r="J607">
-        <v>0.31</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="608">
@@ -27378,7 +27378,7 @@
         <v>3</v>
       </c>
       <c r="J614">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="615">
@@ -27466,7 +27466,7 @@
         <v>3</v>
       </c>
       <c r="J616">
-        <v>0.31</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="617">

</xml_diff>